<commit_message>
made some of the required edits
</commit_message>
<xml_diff>
--- a/Documents/Week5/05_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
+++ b/Documents/Week5/05_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\GitHub\UMGC_495_7381_Work_Request\Documents\Week5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23B857-98F3-43F2-9A97-81647DF93607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="11355" windowHeight="8700"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Traceability Template'!$A$1:$I$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Traceability Template'!$A$1:$J$34</definedName>
     <definedName name="Text2" localSheetId="0">'Traceability Template'!#REF!</definedName>
     <definedName name="Text3" localSheetId="0">'Traceability Template'!#REF!</definedName>
     <definedName name="Text4" localSheetId="0">'Traceability Template'!#REF!</definedName>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Project Name</t>
   </si>
@@ -39,9 +45,6 @@
     <t>Business Area</t>
   </si>
   <si>
-    <t>Business Analyst Lead</t>
-  </si>
-  <si>
     <t>QA Lead</t>
   </si>
   <si>
@@ -54,35 +57,158 @@
     <t>Category/Functional Activity</t>
   </si>
   <si>
-    <t>Design Document Reference</t>
-  </si>
-  <si>
-    <t>Code Module/ Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case Reference </t>
-  </si>
-  <si>
-    <t>User Acceptance Validation</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Requirements Traceability Matrix</t>
   </si>
   <si>
-    <t>Use Case Reference</t>
-  </si>
-  <si>
-    <t>[Company Logo]</t>
+    <t>REQ-001</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Should have</t>
+  </si>
+  <si>
+    <t>Nice to have</t>
+  </si>
+  <si>
+    <t>REQ-002</t>
+  </si>
+  <si>
+    <t>REQ-003</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>CMSC495 Team 3</t>
+  </si>
+  <si>
+    <t>Work Request Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Development </t>
+  </si>
+  <si>
+    <t>Dave Leake</t>
+  </si>
+  <si>
+    <t>Will Tchouente</t>
+  </si>
+  <si>
+    <t>Software Development Lead</t>
+  </si>
+  <si>
+    <t>Ian Oliver</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>The site launches properly with all the relevant pages, features, and logo.</t>
+  </si>
+  <si>
+    <t>user can register/login to the site</t>
+  </si>
+  <si>
+    <t>major functionalities like searching, filtering, etc work as expected</t>
+  </si>
+  <si>
+    <t>Site launches properly in all major browsers</t>
+  </si>
+  <si>
+    <t>user satisfaction from site ease of use</t>
+  </si>
+  <si>
+    <t>REQ-004</t>
+  </si>
+  <si>
+    <t>REQ-005</t>
+  </si>
+  <si>
+    <t>REQ-006</t>
+  </si>
+  <si>
+    <t>REQ-007</t>
+  </si>
+  <si>
+    <t>Content of pages is properly aligned, well managed and without spelling mistakes.</t>
+  </si>
+  <si>
+    <t>REQ-008</t>
+  </si>
+  <si>
+    <t>User can interact with all work requests</t>
+  </si>
+  <si>
+    <t>Session timeout implementation</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Business Need, Justification</t>
+  </si>
+  <si>
+    <t>Application has to be functional for user interaction</t>
+  </si>
+  <si>
+    <t>User has to be able to achieve their goal in using the application</t>
+  </si>
+  <si>
+    <t>for security purpose session must timeout after inactivity</t>
+  </si>
+  <si>
+    <t>User must be able to access application in order to use it</t>
+  </si>
+  <si>
+    <t>application has to be use friendly.</t>
+  </si>
+  <si>
+    <t>application must be functional</t>
+  </si>
+  <si>
+    <t>Project Objective</t>
+  </si>
+  <si>
+    <t>Create Viable application</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Requested by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,7 +260,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,12 +269,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -172,10 +334,142 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -184,17 +478,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -206,15 +494,58 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -222,6 +553,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -268,7 +607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,9 +639,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,6 +691,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,427 +884,619 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.06640625" customWidth="1"/>
+    <col min="2" max="2" width="20.3984375" customWidth="1"/>
+    <col min="3" max="3" width="48.86328125" customWidth="1"/>
+    <col min="4" max="4" width="17.265625" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" customWidth="1"/>
+    <col min="10" max="10" width="25.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
+      <c r="A1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="9" t="s">
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="38.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="6"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="6"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="6"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="6"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -939,8 +1506,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -950,8 +1518,9 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -961,8 +1530,9 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -972,8 +1542,9 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -983,8 +1554,9 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -994,8 +1566,9 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1005,8 +1578,9 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1016,8 +1590,9 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1027,8 +1602,9 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1038,8 +1614,9 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1049,8 +1626,9 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1060,8 +1638,9 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1071,8 +1650,9 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1082,8 +1662,9 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1093,8 +1674,9 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1104,8 +1686,9 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1115,8 +1698,9 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1126,8 +1710,9 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1137,8 +1722,9 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1148,8 +1734,9 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1159,8 +1746,9 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1170,8 +1758,9 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1181,8 +1770,9 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1192,8 +1782,9 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1203,8 +1794,9 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1214,8 +1806,9 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1225,8 +1818,9 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1236,8 +1830,9 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1247,8 +1842,9 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1258,8 +1854,9 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1269,8 +1866,9 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1280,8 +1878,9 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1291,8 +1890,9 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1302,8 +1902,9 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1313,8 +1914,9 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1324,8 +1926,9 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1335,8 +1938,9 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1346,8 +1950,9 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1357,8 +1962,9 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1368,8 +1974,9 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1379,8 +1986,9 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1390,8 +1998,9 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1401,8 +2010,9 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1412,8 +2022,9 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1423,8 +2034,9 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1434,8 +2046,9 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1445,8 +2058,9 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1456,8 +2070,9 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1467,8 +2082,9 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1478,8 +2094,9 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1489,8 +2106,9 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1500,8 +2118,9 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1511,8 +2130,9 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1522,8 +2142,9 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1533,20 +2154,21 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="E1:J1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.55000000000000004" right="0.55000000000000004" top="0.55000000000000004" bottom="0.55000000000000004" header="0.5" footer="0.35"/>

</xml_diff>

<commit_message>
Renamed testdelivery and set target date in the matrix
</commit_message>
<xml_diff>
--- a/Documents/Week5/05_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
+++ b/Documents/Week5/05_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\GitHub\UMGC_495_7381_Work_Request\Documents\Week5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudioRepos\Documents\Week5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23B857-98F3-43F2-9A97-81647DF93607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F304680-2A8F-4A95-B0A3-C9F2EBA7F8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Template" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Project Name</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Ian Oliver</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Test Cases</t>
@@ -494,14 +491,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -512,26 +503,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,6 +521,28 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,372 +888,372 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G4" sqref="G4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" customWidth="1"/>
-    <col min="3" max="3" width="48.86328125" customWidth="1"/>
-    <col min="4" max="4" width="17.265625" customWidth="1"/>
-    <col min="5" max="5" width="19.59765625" customWidth="1"/>
-    <col min="6" max="6" width="18.73046875" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" customWidth="1"/>
-    <col min="10" max="10" width="25.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="18">
+        <v>20211214</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="5">
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" s="3">
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="3">
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="3">
         <v>1004</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="3">
         <v>1005</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="3">
         <v>1006</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="3">
         <v>1007</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="3">
         <v>1008</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1268,7 +1265,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1280,7 +1277,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1292,7 +1289,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1304,7 +1301,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1316,7 +1313,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1328,7 +1325,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1340,7 +1337,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1352,7 +1349,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1364,7 +1361,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1376,7 +1373,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1388,7 +1385,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1400,7 +1397,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1412,7 +1409,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1424,7 +1421,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1436,7 +1433,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1448,7 +1445,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1460,7 +1457,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1472,7 +1469,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1484,7 +1481,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1496,7 +1493,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1508,7 +1505,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1520,7 +1517,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1532,7 +1529,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1544,7 +1541,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1556,7 +1553,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1568,7 +1565,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1580,7 +1577,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1592,7 +1589,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1604,7 +1601,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1616,7 +1613,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1628,7 +1625,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1640,7 +1637,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1652,7 +1649,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1664,7 +1661,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1676,7 +1673,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1688,7 +1685,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1700,7 +1697,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1712,7 +1709,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1724,7 +1721,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1736,7 +1733,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1748,7 +1745,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1760,7 +1757,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1772,7 +1769,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1784,7 +1781,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1796,7 +1793,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1808,7 +1805,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1820,7 +1817,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1832,7 +1829,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1844,7 +1841,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1856,7 +1853,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1868,7 +1865,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1880,7 +1877,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1892,7 +1889,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1904,7 +1901,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1916,7 +1913,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1928,7 +1925,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1940,7 +1937,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1952,7 +1949,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1964,7 +1961,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1976,7 +1973,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1988,7 +1985,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2000,7 +1997,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2012,7 +2009,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2024,7 +2021,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2036,7 +2033,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2048,7 +2045,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2060,7 +2057,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2072,7 +2069,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2084,7 +2081,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2096,7 +2093,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2108,7 +2105,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2120,7 +2117,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2132,7 +2129,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2144,7 +2141,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>

</xml_diff>